<commit_message>
updated method for pulling IeDEA data
</commit_message>
<xml_diff>
--- a/data_manager/IeDEA_data.xlsx
+++ b/data_manager/IeDEA_data.xlsx
@@ -8,15 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissaschnure/Library/CloudStorage/Dropbox/Documents_local/Hopkins/SOM_Job/3_Aging_multimorbidity/gmha/data_manager/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E794BC66-F31C-734B-8392-66F8CAC87145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255DB246-194A-D34E-A34C-1F05BFCECCCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44040" yWindow="4280" windowWidth="16400" windowHeight="14320" activeTab="3" xr2:uid="{78235156-F8DD-3142-BD4C-1F44D370532F}"/>
+    <workbookView xWindow="21960" yWindow="500" windowWidth="16400" windowHeight="14320" activeTab="1" xr2:uid="{78235156-F8DD-3142-BD4C-1F44D370532F}"/>
   </bookViews>
   <sheets>
-    <sheet name="eng_moz" sheetId="1" r:id="rId1"/>
-    <sheet name="supp_moz" sheetId="3" r:id="rId2"/>
-    <sheet name="eng_tanz" sheetId="4" r:id="rId3"/>
-    <sheet name="supp_tanz" sheetId="5" r:id="rId4"/>
+    <sheet name="eng_sa" sheetId="8" r:id="rId1"/>
+    <sheet name="supp_sa" sheetId="9" r:id="rId2"/>
+    <sheet name="eng_ken" sheetId="10" r:id="rId3"/>
+    <sheet name="supp_ken" sheetId="11" r:id="rId4"/>
+    <sheet name="eng_moz" sheetId="1" r:id="rId5"/>
+    <sheet name="supp_moz" sheetId="3" r:id="rId6"/>
+    <sheet name="eng_tanz" sheetId="4" r:id="rId7"/>
+    <sheet name="supp_tanz" sheetId="5" r:id="rId8"/>
+    <sheet name="eng_uga" sheetId="6" r:id="rId9"/>
+    <sheet name="supp_uga" sheetId="7" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="10">
   <si>
     <t>10-19</t>
   </si>
@@ -440,6 +446,1111 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6502D7A-36D4-2C4C-BCF5-6DB0BB05298F}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1990</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2010</v>
+      </c>
+      <c r="B4">
+        <v>0.53</v>
+      </c>
+      <c r="C4">
+        <v>0.54</v>
+      </c>
+      <c r="D4">
+        <v>0.76</v>
+      </c>
+      <c r="E4">
+        <v>0.82</v>
+      </c>
+      <c r="F4">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2014</v>
+      </c>
+      <c r="B5">
+        <v>0.52</v>
+      </c>
+      <c r="C5">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D5">
+        <v>0.71</v>
+      </c>
+      <c r="E5">
+        <v>0.78</v>
+      </c>
+      <c r="F5">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2017</v>
+      </c>
+      <c r="B6">
+        <v>0.91</v>
+      </c>
+      <c r="C6">
+        <v>0.85</v>
+      </c>
+      <c r="D6">
+        <v>0.93</v>
+      </c>
+      <c r="E6">
+        <v>0.94</v>
+      </c>
+      <c r="F6">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1990</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2010</v>
+      </c>
+      <c r="B11">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C11">
+        <v>0.62</v>
+      </c>
+      <c r="D11">
+        <v>0.79</v>
+      </c>
+      <c r="E11">
+        <v>0.79</v>
+      </c>
+      <c r="F11">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2014</v>
+      </c>
+      <c r="B12">
+        <v>0.4</v>
+      </c>
+      <c r="C12">
+        <v>0.65</v>
+      </c>
+      <c r="D12">
+        <v>0.74</v>
+      </c>
+      <c r="E12">
+        <v>0.74</v>
+      </c>
+      <c r="F12">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2017</v>
+      </c>
+      <c r="B13">
+        <v>0.78</v>
+      </c>
+      <c r="C13">
+        <v>0.87</v>
+      </c>
+      <c r="D13">
+        <v>0.91</v>
+      </c>
+      <c r="E13">
+        <v>0.93</v>
+      </c>
+      <c r="F13">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95D3ECD5-5D49-3C4B-A076-68FFEE384AAA}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1990</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2010</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2014</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>0.8</v>
+      </c>
+      <c r="D5">
+        <v>0.79</v>
+      </c>
+      <c r="E5">
+        <v>0.88</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2017</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>0.73</v>
+      </c>
+      <c r="D6">
+        <v>0.82</v>
+      </c>
+      <c r="E6">
+        <v>0.95</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1990</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2010</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2014</v>
+      </c>
+      <c r="B12">
+        <v>0.86</v>
+      </c>
+      <c r="C12">
+        <v>0.88</v>
+      </c>
+      <c r="D12">
+        <v>0.89</v>
+      </c>
+      <c r="E12">
+        <v>0.9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2017</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>0.81</v>
+      </c>
+      <c r="D13">
+        <v>0.8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF35778-5154-3848-9CCA-CB3A649458D5}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1990</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2010</v>
+      </c>
+      <c r="B4">
+        <v>0.76</v>
+      </c>
+      <c r="C4">
+        <v>0.81</v>
+      </c>
+      <c r="D4">
+        <v>0.86</v>
+      </c>
+      <c r="E4">
+        <v>0.85</v>
+      </c>
+      <c r="F4">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2014</v>
+      </c>
+      <c r="B5">
+        <v>0.65</v>
+      </c>
+      <c r="C5">
+        <v>0.88</v>
+      </c>
+      <c r="D5">
+        <v>0.9</v>
+      </c>
+      <c r="E5">
+        <v>0.9</v>
+      </c>
+      <c r="F5">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2017</v>
+      </c>
+      <c r="B6">
+        <v>0.83</v>
+      </c>
+      <c r="C6">
+        <v>0.88</v>
+      </c>
+      <c r="D6">
+        <v>0.87</v>
+      </c>
+      <c r="E6">
+        <v>0.87</v>
+      </c>
+      <c r="F6">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1990</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2010</v>
+      </c>
+      <c r="B11">
+        <v>0.78</v>
+      </c>
+      <c r="C11">
+        <v>0.85</v>
+      </c>
+      <c r="D11">
+        <v>0.88</v>
+      </c>
+      <c r="E11">
+        <v>0.91</v>
+      </c>
+      <c r="F11">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2014</v>
+      </c>
+      <c r="B12">
+        <v>0.87</v>
+      </c>
+      <c r="C12">
+        <v>0.88</v>
+      </c>
+      <c r="D12">
+        <v>0.88</v>
+      </c>
+      <c r="E12">
+        <v>0.91</v>
+      </c>
+      <c r="F12">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2017</v>
+      </c>
+      <c r="B13">
+        <v>0.85</v>
+      </c>
+      <c r="C13">
+        <v>0.86</v>
+      </c>
+      <c r="D13">
+        <v>0.92</v>
+      </c>
+      <c r="E13">
+        <v>0.89</v>
+      </c>
+      <c r="F13">
+        <v>0.96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5FABE65-7922-1242-9229-C4934A3E7CF5}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1990</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2010</v>
+      </c>
+      <c r="B4">
+        <v>0.61</v>
+      </c>
+      <c r="C4">
+        <v>0.45</v>
+      </c>
+      <c r="D4">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E4">
+        <v>0.64</v>
+      </c>
+      <c r="F4">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2014</v>
+      </c>
+      <c r="B5">
+        <v>0.66</v>
+      </c>
+      <c r="C5">
+        <v>0.6</v>
+      </c>
+      <c r="D5">
+        <v>0.7</v>
+      </c>
+      <c r="E5">
+        <v>0.73</v>
+      </c>
+      <c r="F5">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2017</v>
+      </c>
+      <c r="B6">
+        <v>0.86</v>
+      </c>
+      <c r="C6">
+        <v>0.77</v>
+      </c>
+      <c r="D6">
+        <v>0.9</v>
+      </c>
+      <c r="E6">
+        <v>0.92</v>
+      </c>
+      <c r="F6">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1990</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2010</v>
+      </c>
+      <c r="B11">
+        <v>0.37</v>
+      </c>
+      <c r="C11">
+        <v>0.37</v>
+      </c>
+      <c r="D11">
+        <v>0.51</v>
+      </c>
+      <c r="E11">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F11">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2014</v>
+      </c>
+      <c r="B12">
+        <v>0.52</v>
+      </c>
+      <c r="C12">
+        <v>0.5</v>
+      </c>
+      <c r="D12">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E12">
+        <v>0.72</v>
+      </c>
+      <c r="F12">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2017</v>
+      </c>
+      <c r="B13">
+        <v>0.84</v>
+      </c>
+      <c r="C13">
+        <v>0.88</v>
+      </c>
+      <c r="D13">
+        <v>0.91</v>
+      </c>
+      <c r="E13">
+        <v>0.93</v>
+      </c>
+      <c r="F13">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F53371B-1C1C-4747-8EB8-44C9FF6C194B}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1990</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2010</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>0.67</v>
+      </c>
+      <c r="E4">
+        <v>0.69</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2014</v>
+      </c>
+      <c r="B5">
+        <v>0.67</v>
+      </c>
+      <c r="C5">
+        <v>0.67</v>
+      </c>
+      <c r="D5">
+        <v>0.77</v>
+      </c>
+      <c r="E5">
+        <v>0.67</v>
+      </c>
+      <c r="F5">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2017</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>0.73</v>
+      </c>
+      <c r="D6">
+        <v>0.7</v>
+      </c>
+      <c r="E6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F6">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1990</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2010</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>0.52</v>
+      </c>
+      <c r="D11">
+        <v>0.52</v>
+      </c>
+      <c r="E11">
+        <v>0.73</v>
+      </c>
+      <c r="F11">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2014</v>
+      </c>
+      <c r="B12">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C12">
+        <v>0.73</v>
+      </c>
+      <c r="D12">
+        <v>0.66</v>
+      </c>
+      <c r="E12">
+        <v>0.7</v>
+      </c>
+      <c r="F12">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2017</v>
+      </c>
+      <c r="B13">
+        <v>0.49</v>
+      </c>
+      <c r="C13">
+        <v>0.73</v>
+      </c>
+      <c r="D13">
+        <v>0.7</v>
+      </c>
+      <c r="E13">
+        <v>0.7</v>
+      </c>
+      <c r="F13">
+        <v>0.62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA7F01B0-0CA4-494A-807D-2C246F6EC16F}">
   <dimension ref="A1:G13"/>
   <sheetViews>
@@ -676,7 +1787,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0737E4FF-F0BE-2047-89EE-CFC41853E99D}">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -895,7 +2006,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86DE3C10-7BD8-F54F-882B-4D29BA181CAA}">
   <dimension ref="A1:F14"/>
   <sheetViews>
@@ -1122,11 +2233,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED9D9C40-4CE9-AC4E-B169-2F164225CCCB}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -1339,4 +2450,229 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{837DFD6D-BD95-F64B-873B-02C87D96C22D}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1990</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2010</v>
+      </c>
+      <c r="B4">
+        <v>0.39</v>
+      </c>
+      <c r="C4">
+        <v>0.41</v>
+      </c>
+      <c r="D4">
+        <v>0.51</v>
+      </c>
+      <c r="E4">
+        <v>0.52</v>
+      </c>
+      <c r="F4">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2014</v>
+      </c>
+      <c r="B5">
+        <v>0.78</v>
+      </c>
+      <c r="C5">
+        <v>0.84</v>
+      </c>
+      <c r="D5">
+        <v>0.89</v>
+      </c>
+      <c r="E5">
+        <v>0.9</v>
+      </c>
+      <c r="F5">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2017</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>0.95</v>
+      </c>
+      <c r="D6">
+        <v>0.93</v>
+      </c>
+      <c r="E6">
+        <v>0.96</v>
+      </c>
+      <c r="F6">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1990</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2010</v>
+      </c>
+      <c r="B11">
+        <v>0.35</v>
+      </c>
+      <c r="C11">
+        <v>0.41</v>
+      </c>
+      <c r="D11">
+        <v>0.46</v>
+      </c>
+      <c r="E11">
+        <v>0.5</v>
+      </c>
+      <c r="F11">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2014</v>
+      </c>
+      <c r="B12">
+        <v>0.77</v>
+      </c>
+      <c r="C12">
+        <v>0.76</v>
+      </c>
+      <c r="D12">
+        <v>0.81</v>
+      </c>
+      <c r="E12">
+        <v>0.86</v>
+      </c>
+      <c r="F12">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2017</v>
+      </c>
+      <c r="B13">
+        <v>0.77</v>
+      </c>
+      <c r="C13">
+        <v>0.79</v>
+      </c>
+      <c r="D13">
+        <v>0.89</v>
+      </c>
+      <c r="E13">
+        <v>0.97</v>
+      </c>
+      <c r="F13">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added zambia and zimbabwe
</commit_message>
<xml_diff>
--- a/data_manager/IeDEA_data.xlsx
+++ b/data_manager/IeDEA_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissaschnure/Library/CloudStorage/Dropbox/Documents_local/Hopkins/SOM_Job/3_Aging_multimorbidity/gmha/data_manager/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255DB246-194A-D34E-A34C-1F05BFCECCCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EE0FE2-01E9-524C-8FB8-40363B1CFA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21960" yWindow="500" windowWidth="16400" windowHeight="14320" activeTab="1" xr2:uid="{78235156-F8DD-3142-BD4C-1F44D370532F}"/>
+    <workbookView xWindow="20800" yWindow="500" windowWidth="17560" windowHeight="19540" firstSheet="6" activeTab="13" xr2:uid="{78235156-F8DD-3142-BD4C-1F44D370532F}"/>
   </bookViews>
   <sheets>
     <sheet name="eng_sa" sheetId="8" r:id="rId1"/>
@@ -23,6 +23,10 @@
     <sheet name="supp_tanz" sheetId="5" r:id="rId8"/>
     <sheet name="eng_uga" sheetId="6" r:id="rId9"/>
     <sheet name="supp_uga" sheetId="7" r:id="rId10"/>
+    <sheet name="eng_zam" sheetId="12" r:id="rId11"/>
+    <sheet name="supp_zam" sheetId="13" r:id="rId12"/>
+    <sheet name="eng_zim" sheetId="14" r:id="rId13"/>
+    <sheet name="supp_zim" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -45,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="10">
   <si>
     <t>10-19</t>
   </si>
@@ -887,11 +891,903 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B0A3F1-1990-2D42-95F5-430294AC3DC8}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1990</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2010</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2014</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2017</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1990</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2010</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2014</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2017</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B489BF32-33AD-9C4B-A3FB-46655CC77E21}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1990</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2010</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2014</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2017</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1990</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2010</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2014</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2017</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{026438C9-7687-E64B-9D7E-9D28B576C154}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1990</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2010</v>
+      </c>
+      <c r="B4">
+        <v>0.96</v>
+      </c>
+      <c r="C4">
+        <v>0.96</v>
+      </c>
+      <c r="D4">
+        <v>0.97</v>
+      </c>
+      <c r="E4">
+        <v>0.98</v>
+      </c>
+      <c r="F4">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2014</v>
+      </c>
+      <c r="B5">
+        <v>0.96</v>
+      </c>
+      <c r="C5">
+        <v>0.97</v>
+      </c>
+      <c r="D5">
+        <v>0.98</v>
+      </c>
+      <c r="E5">
+        <v>0.96</v>
+      </c>
+      <c r="F5">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2017</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>0.98</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1990</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2010</v>
+      </c>
+      <c r="B11">
+        <v>0.89</v>
+      </c>
+      <c r="C11">
+        <v>0.95</v>
+      </c>
+      <c r="D11">
+        <v>0.98</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2014</v>
+      </c>
+      <c r="B12">
+        <v>0.96</v>
+      </c>
+      <c r="C12">
+        <v>0.99</v>
+      </c>
+      <c r="D12">
+        <v>0.98</v>
+      </c>
+      <c r="E12">
+        <v>0.98</v>
+      </c>
+      <c r="F12">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2017</v>
+      </c>
+      <c r="B13">
+        <v>0.95</v>
+      </c>
+      <c r="C13">
+        <v>0.99</v>
+      </c>
+      <c r="D13">
+        <v>0.99</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC8890B-5B8E-9646-80E9-5F9397CAEDD8}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1990</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2010</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2014</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2017</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1990</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2010</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2014</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>0.94</v>
+      </c>
+      <c r="D12">
+        <v>0.9</v>
+      </c>
+      <c r="E12">
+        <v>0.95</v>
+      </c>
+      <c r="F12">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2017</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF35778-5154-3848-9CCA-CB3A649458D5}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>

</xml_diff>